<commit_message>
using gains for all
</commit_message>
<xml_diff>
--- a/Sep19/pos_prof/Tables/groups-M.xlsx
+++ b/Sep19/pos_prof/Tables/groups-M.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>M_ETR</t>
   </si>
@@ -26,6 +26,12 @@
   </si>
   <si>
     <t>M_POP</t>
+  </si>
+  <si>
+    <t>M_TotalTax</t>
+  </si>
+  <si>
+    <t>M_CorpTax</t>
   </si>
   <si>
     <t>GFA - Sales</t>
@@ -440,15 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -486,10 +492,16 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>0.2016509700010976</v>
@@ -504,33 +516,39 @@
         <v>505635568.25</v>
       </c>
       <c r="F2">
+        <v>6308727034979.312</v>
+      </c>
+      <c r="G2">
+        <v>399825921028.5854</v>
+      </c>
+      <c r="H2">
         <v>37914254851.3345</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>27187746519.70345</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>21002851541.16861</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>13796697370.0489</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>5094219988.365887</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>3652989154.141948</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>25471099941.82938</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>18264945770.70968</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>0.2213307288476244</v>
@@ -545,33 +563,39 @@
         <v>4474178143.75</v>
       </c>
       <c r="F3">
+        <v>16630145391623.02</v>
+      </c>
+      <c r="G3">
+        <v>1639742485782.957</v>
+      </c>
+      <c r="H3">
         <v>126851392957.2347</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>172895313356.448</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>136070479393.6599</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>167003153734.7653</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>17043956266.28165</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>23230491134.50268</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>85219781331.40788</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>116152455672.5132</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>0.3720453617170856</v>
@@ -586,33 +610,39 @@
         <v>3433428530.25</v>
       </c>
       <c r="F4">
+        <v>4450994137606.095</v>
+      </c>
+      <c r="G4">
+        <v>601350231413.5104</v>
+      </c>
+      <c r="H4">
         <v>11740879900.00649</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>68212219683.54447</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>9743440338.087193</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>47681338501.0752</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>1577523422.31542</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>9165103054.913021</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>7887617111.577099</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>45825515274.56509</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>0.439636374826367</v>
@@ -627,33 +657,39 @@
         <v>3959384333.5</v>
       </c>
       <c r="F5">
+        <v>4183547438952.192</v>
+      </c>
+      <c r="G5">
+        <v>598849276038.3025</v>
+      </c>
+      <c r="H5">
         <v>17628533204.04444</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>96300212885.54436</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>16460388674.8146</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>69312652912.00934</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>2368597947.282457</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>12939050794.72141</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>11842989736.41228</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>64695253973.60701</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>0.2096734066447806</v>
@@ -668,33 +704,39 @@
         <v>759996120.5</v>
       </c>
       <c r="F6">
+        <v>11223287075501.79</v>
+      </c>
+      <c r="G6">
+        <v>872292028558.4308</v>
+      </c>
+      <c r="H6">
         <v>101726216980.6352</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>71124767909.86188</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>109531351177.2212</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>88973052703.39453</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>13668097392.80314</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>9556437698.037764</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>68340486964.01531</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>47782188490.18865</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>0.387039958292552</v>
@@ -709,33 +751,39 @@
         <v>3118581654.5</v>
       </c>
       <c r="F7">
+        <v>1841737275230.086</v>
+      </c>
+      <c r="G7">
+        <v>214321200777.9413</v>
+      </c>
+      <c r="H7">
         <v>4511707797.04856</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>59581986765.36914</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>8008750089.676789</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>45005404380.43485</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>606200283.5480216</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>8005531141.69963</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>3031001417.74011</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>40027655708.49816</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>0.2684919396530561</v>
@@ -750,33 +798,39 @@
         <v>437799251.25</v>
       </c>
       <c r="F8">
+        <v>6192585801479.285</v>
+      </c>
+      <c r="G8">
+        <v>516695167857.3162</v>
+      </c>
+      <c r="H8">
         <v>50935450591.94768</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>57494585238.23689</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>43463691892.87671</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>47870171059.15968</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>6843768697.007366</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>7725064530.263959</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>34218843485.0368</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>38625322651.31976</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>0.2116872184609259</v>
@@ -791,33 +845,39 @@
         <v>1279357787</v>
       </c>
       <c r="F9">
+        <v>14653861967257.56</v>
+      </c>
+      <c r="G9">
+        <v>1232540278767.842</v>
+      </c>
+      <c r="H9">
         <v>107294496669.7625</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>83196889524.47711</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>109567407543.8588</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>93378442143.82013</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>14416260367.50462</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>11178467287.49684</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>72081301837.52269</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>55892336437.48399</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>0.2458369632575438</v>
@@ -832,33 +892,39 @@
         <v>957160917.75</v>
       </c>
       <c r="F10">
+        <v>9623160693235.053</v>
+      </c>
+      <c r="G10">
+        <v>876943418066.7275</v>
+      </c>
+      <c r="H10">
         <v>56503730281.07501</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>69566706852.85211</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>43499748259.51436</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>52275560499.58531</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>7591931671.708843</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>9347094119.723038</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>37959658358.54415</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>46735470598.61511</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>0.2034671187804626</v>
@@ -873,27 +939,33 @@
         <v>322196869.25</v>
       </c>
       <c r="F11">
+        <v>5030701274022.499</v>
+      </c>
+      <c r="G11">
+        <v>355596860701.1148</v>
+      </c>
+      <c r="H11">
         <v>50790766388.6875</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>13630182671.625</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>66067659284.34447</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>41102881644.23486</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>6824328695.795775</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>1831373167.773804</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>34121643478.97852</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>9156865838.868895</v>
       </c>
     </row>

</xml_diff>